<commit_message>
some updates post receiving the SCADAhacker material
</commit_message>
<xml_diff>
--- a/Categorization.xlsx
+++ b/Categorization.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="201">
   <si/>
   <si>
     <t>Topic Coverage</t>
@@ -108,6 +108,9 @@
     <t>Control System Background</t>
   </si>
   <si>
+    <t>Controls for addressing risk</t>
+  </si>
+  <si>
     <t>Controller and Field Device Security</t>
   </si>
   <si>
@@ -150,9 +153,6 @@
     <t>Firmware exploitiation</t>
   </si>
   <si>
-    <t>Follows assessment methodology</t>
-  </si>
-  <si>
     <t>Forensics</t>
   </si>
   <si>
@@ -264,6 +264,9 @@
     <t>Network Fundamentals</t>
   </si>
   <si>
+    <t>Network Security</t>
+  </si>
+  <si>
     <t>Online course option</t>
   </si>
   <si>
@@ -312,6 +315,9 @@
     <t>Risk Assessment and Auditing</t>
   </si>
   <si>
+    <t>Risk Assessment Tools (e.g., CSET)</t>
+  </si>
+  <si>
     <t>Secure DCS Architecture</t>
   </si>
   <si>
@@ -330,6 +336,9 @@
     <t>Standards and Best Practices</t>
   </si>
   <si>
+    <t>System characterization example</t>
+  </si>
+  <si>
     <t>Takeaway hands-on hardware (links or equipment)</t>
   </si>
   <si>
@@ -345,7 +354,7 @@
     <t>TCP/IP middle-layers</t>
   </si>
   <si>
-    <t>Teaches how to use openly available tools</t>
+    <t>Teaches how to use openly available security tools</t>
   </si>
   <si>
     <t>Teaches control system context</t>
@@ -813,7 +822,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Topic Coverage - Topic Coverage'!$A$112</c:f>
+              <c:f>'Topic Coverage - Topic Coverage'!$A$115</c:f>
               <c:strCache>
                 <c:pt idx="0">
                   <c:v>Percentage</c:v>
@@ -908,23 +917,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Topic Coverage - Topic Coverage'!$B$112:$F$112</c:f>
+              <c:f>'Topic Coverage - Topic Coverage'!$B$115:$F$115</c:f>
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.697248</c:v>
+                  <c:v>0.687500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.550459</c:v>
+                  <c:v>0.526786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.587156</c:v>
+                  <c:v>0.589286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.587156</c:v>
+                  <c:v>0.589286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.183486</c:v>
+                  <c:v>0.178571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1234,7 +1243,7 @@
                   <c:v>0.727273</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.636364</c:v>
+                  <c:v>0.727273</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.000000</c:v>
@@ -1547,7 +1556,7 @@
                   <c:v>0.714286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.571429</c:v>
+                  <c:v>0.714286</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.142857</c:v>
@@ -1851,7 +1860,7 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.450000</c:v>
+                  <c:v>0.433333</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.250000</c:v>
@@ -1860,10 +1869,10 @@
                   <c:v>0.450000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.350000</c:v>
+                  <c:v>0.333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.250000</c:v>
+                  <c:v>0.266667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2031,14 +2040,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>241111</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>200034</xdr:rowOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>200030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>255075</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>123834</xdr:rowOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>123830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2046,8 +2055,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="241111" y="29841825"/>
-        <a:ext cx="5115317" cy="3810000"/>
+        <a:off x="241111" y="30617159"/>
+        <a:ext cx="5115317" cy="3810001"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3391,7 +3400,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F113"/>
+  <dimension ref="A2:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
@@ -3604,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b" s="6">
         <v>0</v>
@@ -3624,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b" s="6">
         <v>1</v>
@@ -3890,7 +3899,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="b" s="6">
         <v>0</v>
@@ -3924,7 +3933,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b" s="6">
         <v>1</v>
@@ -3941,7 +3950,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" t="b" s="6">
         <v>1</v>
@@ -3953,7 +3962,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" ht="20.35" customHeight="1">
@@ -3961,19 +3970,19 @@
         <v>33</v>
       </c>
       <c r="B29" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="b" s="6">
         <v>1</v>
       </c>
       <c r="E29" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="20.35" customHeight="1">
@@ -3984,7 +3993,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b" s="6">
         <v>1</v>
@@ -4001,7 +4010,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" t="b" s="6">
         <v>1</v>
@@ -4010,7 +4019,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="b" s="6">
         <v>0</v>
@@ -4027,7 +4036,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="b" s="6">
         <v>0</v>
@@ -4044,13 +4053,13 @@
         <v>0</v>
       </c>
       <c r="C33" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="b" s="6">
         <v>0</v>
@@ -4061,16 +4070,16 @@
         <v>38</v>
       </c>
       <c r="B34" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="b" s="6">
         <v>0</v>
       </c>
       <c r="D34" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="b" s="6">
         <v>0</v>
@@ -4087,13 +4096,13 @@
         <v>0</v>
       </c>
       <c r="D35" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="20.35" customHeight="1">
@@ -4104,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="b" s="6">
         <v>1</v>
@@ -4113,7 +4122,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" ht="20.35" customHeight="1">
@@ -4124,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="b" s="6">
         <v>1</v>
@@ -4133,7 +4142,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="20.35" customHeight="1">
@@ -4144,16 +4153,16 @@
         <v>1</v>
       </c>
       <c r="C38" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" ht="20.35" customHeight="1">
@@ -4181,7 +4190,7 @@
         <v>44</v>
       </c>
       <c r="B40" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="b" s="6">
         <v>1</v>
@@ -4201,7 +4210,7 @@
         <v>45</v>
       </c>
       <c r="B41" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="b" s="6">
         <v>1</v>
@@ -4210,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="b" s="6">
         <v>0</v>
@@ -4410,7 +4419,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="b" s="6">
         <v>0</v>
@@ -4964,13 +4973,13 @@
         <v>1</v>
       </c>
       <c r="C79" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" t="b" s="6">
         <v>0</v>
@@ -5007,7 +5016,7 @@
         <v>1</v>
       </c>
       <c r="D81" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" t="b" s="6">
         <v>0</v>
@@ -5021,10 +5030,10 @@
         <v>86</v>
       </c>
       <c r="B82" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" t="b" s="6">
         <v>1</v>
@@ -5050,7 +5059,7 @@
         <v>1</v>
       </c>
       <c r="E83" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="b" s="6">
         <v>0</v>
@@ -5064,13 +5073,13 @@
         <v>0</v>
       </c>
       <c r="C84" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" t="b" s="6">
         <v>0</v>
@@ -5081,16 +5090,16 @@
         <v>89</v>
       </c>
       <c r="B85" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" t="b" s="6">
         <v>0</v>
@@ -5104,10 +5113,10 @@
         <v>1</v>
       </c>
       <c r="C86" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" t="b" s="6">
         <v>1</v>
@@ -5124,13 +5133,13 @@
         <v>1</v>
       </c>
       <c r="C87" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" t="b" s="6">
         <v>0</v>
       </c>
       <c r="E87" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="b" s="6">
         <v>0</v>
@@ -5144,13 +5153,13 @@
         <v>1</v>
       </c>
       <c r="C88" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" t="b" s="6">
         <v>0</v>
       </c>
       <c r="E88" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" t="b" s="6">
         <v>0</v>
@@ -5164,13 +5173,13 @@
         <v>1</v>
       </c>
       <c r="C89" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89" t="b" s="6">
         <v>0</v>
       </c>
       <c r="E89" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="b" s="6">
         <v>0</v>
@@ -5190,10 +5199,10 @@
         <v>0</v>
       </c>
       <c r="E90" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" ht="20.35" customHeight="1">
@@ -5204,16 +5213,16 @@
         <v>1</v>
       </c>
       <c r="C91" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" t="b" s="6">
         <v>1</v>
       </c>
       <c r="F91" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" ht="20.35" customHeight="1">
@@ -5221,16 +5230,16 @@
         <v>96</v>
       </c>
       <c r="B92" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" t="b" s="6">
         <v>1</v>
       </c>
       <c r="D92" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" t="b" s="6">
         <v>0</v>
@@ -5261,16 +5270,16 @@
         <v>98</v>
       </c>
       <c r="B94" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" t="b" s="6">
         <v>0</v>
@@ -5307,7 +5316,7 @@
         <v>0</v>
       </c>
       <c r="D96" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="b" s="6">
         <v>1</v>
@@ -5321,16 +5330,16 @@
         <v>101</v>
       </c>
       <c r="B97" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" t="b" s="6">
         <v>0</v>
@@ -5341,16 +5350,16 @@
         <v>102</v>
       </c>
       <c r="B98" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" t="b" s="6">
         <v>0</v>
@@ -5367,7 +5376,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="b" s="6">
         <v>0</v>
@@ -5384,13 +5393,13 @@
         <v>1</v>
       </c>
       <c r="C100" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100" t="b" s="6">
         <v>0</v>
       </c>
       <c r="E100" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" t="b" s="6">
         <v>0</v>
@@ -5401,13 +5410,13 @@
         <v>105</v>
       </c>
       <c r="B101" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" t="b" s="6">
         <v>1</v>
       </c>
       <c r="D101" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" t="b" s="6">
         <v>0</v>
@@ -5424,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="C102" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102" t="b" s="6">
         <v>0</v>
@@ -5441,13 +5450,13 @@
         <v>107</v>
       </c>
       <c r="B103" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" t="b" s="6">
         <v>1</v>
@@ -5467,13 +5476,13 @@
         <v>1</v>
       </c>
       <c r="D104" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" t="b" s="6">
         <v>0</v>
       </c>
       <c r="F104" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" ht="20.35" customHeight="1">
@@ -5487,13 +5496,13 @@
         <v>1</v>
       </c>
       <c r="D105" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" ht="20.35" customHeight="1">
@@ -5524,16 +5533,16 @@
         <v>1</v>
       </c>
       <c r="C107" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" t="b" s="6">
         <v>1</v>
       </c>
       <c r="E107" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" ht="20.35" customHeight="1">
@@ -5541,10 +5550,10 @@
         <v>112</v>
       </c>
       <c r="B108" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108" t="b" s="6">
         <v>1</v>
@@ -5553,7 +5562,7 @@
         <v>0</v>
       </c>
       <c r="F108" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" ht="20.35" customHeight="1">
@@ -5567,7 +5576,7 @@
         <v>1</v>
       </c>
       <c r="D109" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="b" s="6">
         <v>1</v>
@@ -5581,7 +5590,7 @@
         <v>114</v>
       </c>
       <c r="B110" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C110" t="b" s="6">
         <v>0</v>
@@ -5590,18 +5599,18 @@
         <v>1</v>
       </c>
       <c r="E110" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" t="b" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="111" ht="20.55" customHeight="1">
+    <row r="111" ht="20.35" customHeight="1">
       <c r="A111" t="s" s="5">
         <v>115</v>
       </c>
       <c r="B111" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" t="b" s="6">
         <v>0</v>
@@ -5616,53 +5625,113 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" ht="20.55" customHeight="1">
-      <c r="A112" t="s" s="7">
+    <row r="112" ht="20.35" customHeight="1">
+      <c r="A112" t="s" s="5">
         <v>116</v>
       </c>
-      <c r="B112" s="8">
-        <f>COUNTIF(B3:B111,TRUE)/COUNTA(B3:B111)</f>
-        <v>0.6972477064220184</v>
-      </c>
-      <c r="C112" s="8">
-        <f>COUNTIF(C3:C111,TRUE)/COUNTA(C3:C111)</f>
-        <v>0.5504587155963303</v>
-      </c>
-      <c r="D112" s="8">
-        <f>COUNTIF(D3:D111,TRUE)/COUNTA(D3:D111)</f>
-        <v>0.5871559633027523</v>
-      </c>
-      <c r="E112" s="8">
-        <f>COUNTIF(E3:E111,TRUE)/COUNTA(E3:E111)</f>
-        <v>0.5871559633027523</v>
-      </c>
-      <c r="F112" s="8">
-        <f>COUNTIF(F3:F111,TRUE)/COUNTA(F3:F111)</f>
-        <v>0.1834862385321101</v>
+      <c r="B112" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="C112" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="D112" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="F112" t="b" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="113" ht="20.35" customHeight="1">
-      <c r="A113" t="s" s="7">
+      <c r="A113" t="s" s="5">
         <v>117</v>
       </c>
-      <c r="B113" s="7">
-        <f>COUNTIF(B2:B111,TRUE)</f>
-        <v>76</v>
-      </c>
-      <c r="C113" s="7">
-        <f>COUNTIF(C2:C111,TRUE)</f>
-        <v>60</v>
-      </c>
-      <c r="D113" s="7">
-        <f>COUNTIF(D2:D111,TRUE)</f>
-        <v>64</v>
-      </c>
-      <c r="E113" s="7">
-        <f>COUNTIF(E2:E111,TRUE)</f>
-        <v>64</v>
-      </c>
-      <c r="F113" s="7">
-        <f>COUNTIF(F2:F111,TRUE)</f>
+      <c r="B113" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="C113" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="D113" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="E113" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="F113" t="b" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" ht="20.55" customHeight="1">
+      <c r="A114" t="s" s="5">
+        <v>118</v>
+      </c>
+      <c r="B114" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="C114" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="D114" t="b" s="6">
+        <v>1</v>
+      </c>
+      <c r="E114" t="b" s="6">
+        <v>0</v>
+      </c>
+      <c r="F114" t="b" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" ht="20.55" customHeight="1">
+      <c r="A115" t="s" s="7">
+        <v>119</v>
+      </c>
+      <c r="B115" s="8">
+        <f>COUNTIF(B3:B114,TRUE)/COUNTA(B3:B114)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="C115" s="8">
+        <f>COUNTIF(C3:C114,TRUE)/COUNTA(C3:C114)</f>
+        <v>0.5267857142857143</v>
+      </c>
+      <c r="D115" s="8">
+        <f>COUNTIF(D3:D114,TRUE)/COUNTA(D3:D114)</f>
+        <v>0.5892857142857143</v>
+      </c>
+      <c r="E115" s="8">
+        <f>COUNTIF(E3:E114,TRUE)/COUNTA(E3:E114)</f>
+        <v>0.5892857142857143</v>
+      </c>
+      <c r="F115" s="8">
+        <f>COUNTIF(F3:F114,TRUE)/COUNTA(F3:F114)</f>
+        <v>0.1785714285714286</v>
+      </c>
+    </row>
+    <row r="116" ht="20.35" customHeight="1">
+      <c r="A116" t="s" s="7">
+        <v>120</v>
+      </c>
+      <c r="B116" s="7">
+        <f>COUNTIF(B2:B114,TRUE)</f>
+        <v>77</v>
+      </c>
+      <c r="C116" s="7">
+        <f>COUNTIF(C2:C114,TRUE)</f>
+        <v>59</v>
+      </c>
+      <c r="D116" s="7">
+        <f>COUNTIF(D2:D114,TRUE)</f>
+        <v>66</v>
+      </c>
+      <c r="E116" s="7">
+        <f>COUNTIF(E2:E114,TRUE)</f>
+        <v>66</v>
+      </c>
+      <c r="F116" s="7">
+        <f>COUNTIF(F2:F114,TRUE)</f>
         <v>20</v>
       </c>
     </row>
@@ -5706,7 +5775,7 @@
     <row r="1" ht="2" customHeight="1"/>
     <row r="2">
       <c r="B2" t="s" s="2">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -5734,7 +5803,7 @@
     </row>
     <row r="4" ht="20.55" customHeight="1">
       <c r="B4" t="s" s="5">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C4" t="b" s="6">
         <v>1</v>
@@ -5754,7 +5823,7 @@
     </row>
     <row r="5" ht="20.35" customHeight="1">
       <c r="B5" t="s" s="5">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C5" t="b" s="10">
         <v>1</v>
@@ -5774,7 +5843,7 @@
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="B6" t="s" s="5">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C6" t="b" s="6">
         <v>1</v>
@@ -5794,7 +5863,7 @@
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="B7" t="s" s="5">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C7" t="b" s="10">
         <v>1</v>
@@ -5814,7 +5883,7 @@
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="B8" t="s" s="5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C8" t="b" s="6">
         <v>1</v>
@@ -5834,7 +5903,7 @@
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="B9" t="s" s="5">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C9" t="b" s="10">
         <v>1</v>
@@ -5854,7 +5923,7 @@
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="B10" t="s" s="5">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C10" t="b" s="6">
         <v>1</v>
@@ -5866,7 +5935,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="b" s="6">
         <v>0</v>
@@ -5874,7 +5943,7 @@
     </row>
     <row r="11" ht="20.35" customHeight="1">
       <c r="B11" t="s" s="5">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C11" t="b" s="10">
         <v>1</v>
@@ -5894,7 +5963,7 @@
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="B12" t="s" s="5">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C12" t="b" s="6">
         <v>0</v>
@@ -5914,7 +5983,7 @@
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="B13" t="s" s="5">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C13" t="b" s="10">
         <v>1</v>
@@ -5934,7 +6003,7 @@
     </row>
     <row r="14" ht="20.55" customHeight="1">
       <c r="B14" t="s" s="5">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C14" t="b" s="6">
         <v>1</v>
@@ -5954,7 +6023,7 @@
     </row>
     <row r="15" ht="20.55" customHeight="1">
       <c r="B15" t="s" s="7">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(C4:C14,TRUE)/COUNTA(C4:C14)</f>
@@ -5970,7 +6039,7 @@
       </c>
       <c r="F15" s="8">
         <f>COUNTIF(F4:F14,TRUE)/COUNTA(F4:F14)</f>
-        <v>0.6363636363636364</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G15" s="8">
         <f>COUNTIF(G4:G14,TRUE)/COUNTA(G4:G14)</f>
@@ -5979,7 +6048,7 @@
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="B16" t="s" s="7">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C16" s="7">
         <f>COUNTIF(C4:C14,TRUE)</f>
@@ -5995,7 +6064,7 @@
       </c>
       <c r="F16" s="7">
         <f>COUNTIF(F4:F14,TRUE)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G16" s="7">
         <f>COUNTIF(G4:G14,TRUE)</f>
@@ -6042,7 +6111,7 @@
     <row r="1" ht="2" customHeight="1"/>
     <row r="2">
       <c r="B2" t="s" s="2">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -6070,7 +6139,7 @@
     </row>
     <row r="4" ht="176.55" customHeight="1">
       <c r="B4" t="s" s="5">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C4" t="b" s="6">
         <v>0</v>
@@ -6090,7 +6159,7 @@
     </row>
     <row r="5" ht="188.35" customHeight="1">
       <c r="B5" t="s" s="5">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C5" t="b" s="10">
         <v>1</v>
@@ -6110,7 +6179,7 @@
     </row>
     <row r="6" ht="140.35" customHeight="1">
       <c r="B6" t="s" s="5">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C6" t="b" s="6">
         <v>1</v>
@@ -6130,7 +6199,7 @@
     </row>
     <row r="7" ht="140.35" customHeight="1">
       <c r="B7" t="s" s="5">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C7" t="b" s="10">
         <v>1</v>
@@ -6150,7 +6219,7 @@
     </row>
     <row r="8" ht="164.35" customHeight="1">
       <c r="B8" t="s" s="5">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C8" t="b" s="6">
         <v>1</v>
@@ -6162,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b" s="6">
         <v>0</v>
@@ -6170,7 +6239,7 @@
     </row>
     <row r="9" ht="140.35" customHeight="1">
       <c r="B9" t="s" s="5">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C9" t="b" s="10">
         <v>1</v>
@@ -6190,7 +6259,7 @@
     </row>
     <row r="10" ht="188.55" customHeight="1">
       <c r="B10" t="s" s="5">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C10" t="b" s="6">
         <v>1</v>
@@ -6210,7 +6279,7 @@
     </row>
     <row r="11" ht="20.55" customHeight="1">
       <c r="B11" t="s" s="7">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C11" s="8">
         <f>COUNTIF(C4:C10,TRUE)/COUNTA(C4:C10)</f>
@@ -6226,7 +6295,7 @@
       </c>
       <c r="F11" s="8">
         <f>COUNTIF(F4:F10,TRUE)/COUNTA(F4:F10)</f>
-        <v>0.5714285714285714</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G11" s="8">
         <f>COUNTIF(G4:G10,TRUE)/COUNTA(G4:G10)</f>
@@ -6235,7 +6304,7 @@
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="B12" t="s" s="7">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C12" s="7">
         <f>COUNTIF(C4:C10,TRUE)</f>
@@ -6251,7 +6320,7 @@
       </c>
       <c r="F12" s="7">
         <f>COUNTIF(F4:F10,TRUE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12" s="7">
         <f>COUNTIF(G4:G10,TRUE)</f>
@@ -6298,7 +6367,7 @@
     <row r="1" ht="2" customHeight="1"/>
     <row r="2">
       <c r="B2" t="s" s="2">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -6326,7 +6395,7 @@
     </row>
     <row r="4" ht="32.55" customHeight="1">
       <c r="B4" t="s" s="5">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C4" t="b" s="6">
         <v>0</v>
@@ -6346,7 +6415,7 @@
     </row>
     <row r="5" ht="32.35" customHeight="1">
       <c r="B5" t="s" s="5">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C5" t="b" s="10">
         <v>1</v>
@@ -6366,7 +6435,7 @@
     </row>
     <row r="6" ht="32.35" customHeight="1">
       <c r="B6" t="s" s="5">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C6" t="b" s="6">
         <v>1</v>
@@ -6386,7 +6455,7 @@
     </row>
     <row r="7" ht="32.35" customHeight="1">
       <c r="B7" t="s" s="5">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C7" t="b" s="10">
         <v>1</v>
@@ -6406,7 +6475,7 @@
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="B8" t="s" s="5">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C8" t="b" s="6">
         <v>1</v>
@@ -6426,7 +6495,7 @@
     </row>
     <row r="9" ht="32.35" customHeight="1">
       <c r="B9" t="s" s="5">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C9" t="b" s="10">
         <v>1</v>
@@ -6446,7 +6515,7 @@
     </row>
     <row r="10" ht="32.35" customHeight="1">
       <c r="B10" t="s" s="5">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C10" t="b" s="6">
         <v>1</v>
@@ -6466,7 +6535,7 @@
     </row>
     <row r="11" ht="32.35" customHeight="1">
       <c r="B11" t="s" s="5">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C11" t="b" s="10">
         <v>0</v>
@@ -6486,7 +6555,7 @@
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="B12" t="s" s="5">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C12" t="b" s="6">
         <v>0</v>
@@ -6506,7 +6575,7 @@
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="B13" t="s" s="5">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C13" t="b" s="10">
         <v>0</v>
@@ -6518,7 +6587,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="b" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b" s="10">
         <v>1</v>
@@ -6526,7 +6595,7 @@
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="B14" t="s" s="5">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C14" t="b" s="6">
         <v>0</v>
@@ -6546,7 +6615,7 @@
     </row>
     <row r="15" ht="32.35" customHeight="1">
       <c r="B15" t="s" s="5">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C15" t="b" s="10">
         <v>0</v>
@@ -6566,7 +6635,7 @@
     </row>
     <row r="16" ht="44.35" customHeight="1">
       <c r="B16" t="s" s="5">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C16" t="b" s="6">
         <v>0</v>
@@ -6586,7 +6655,7 @@
     </row>
     <row r="17" ht="32.35" customHeight="1">
       <c r="B17" t="s" s="5">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C17" t="b" s="10">
         <v>1</v>
@@ -6606,7 +6675,7 @@
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="B18" t="s" s="5">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C18" t="b" s="6">
         <v>1</v>
@@ -6618,7 +6687,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b" s="6">
         <v>1</v>
@@ -6626,7 +6695,7 @@
     </row>
     <row r="19" ht="32.35" customHeight="1">
       <c r="B19" t="s" s="5">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C19" t="b" s="10">
         <v>1</v>
@@ -6646,7 +6715,7 @@
     </row>
     <row r="20" ht="32.35" customHeight="1">
       <c r="B20" t="s" s="5">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C20" t="b" s="6">
         <v>0</v>
@@ -6686,7 +6755,7 @@
     </row>
     <row r="22" ht="20.35" customHeight="1">
       <c r="B22" t="s" s="5">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C22" t="b" s="6">
         <v>1</v>
@@ -6706,7 +6775,7 @@
     </row>
     <row r="23" ht="32.35" customHeight="1">
       <c r="B23" t="s" s="5">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C23" t="b" s="10">
         <v>1</v>
@@ -6726,7 +6795,7 @@
     </row>
     <row r="24" ht="20.35" customHeight="1">
       <c r="B24" t="s" s="5">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C24" t="b" s="6">
         <v>1</v>
@@ -6746,7 +6815,7 @@
     </row>
     <row r="25" ht="32.35" customHeight="1">
       <c r="B25" t="s" s="5">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C25" t="b" s="10">
         <v>0</v>
@@ -6766,7 +6835,7 @@
     </row>
     <row r="26" ht="32.35" customHeight="1">
       <c r="B26" t="s" s="5">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C26" t="b" s="6">
         <v>1</v>
@@ -6786,7 +6855,7 @@
     </row>
     <row r="27" ht="32.35" customHeight="1">
       <c r="B27" t="s" s="5">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C27" t="b" s="10">
         <v>1</v>
@@ -6806,7 +6875,7 @@
     </row>
     <row r="28" ht="32.35" customHeight="1">
       <c r="B28" t="s" s="5">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C28" t="b" s="6">
         <v>0</v>
@@ -6826,7 +6895,7 @@
     </row>
     <row r="29" ht="44.35" customHeight="1">
       <c r="B29" t="s" s="5">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C29" t="b" s="10">
         <v>0</v>
@@ -6846,7 +6915,7 @@
     </row>
     <row r="30" ht="44.35" customHeight="1">
       <c r="B30" t="s" s="5">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C30" t="b" s="6">
         <v>1</v>
@@ -6866,7 +6935,7 @@
     </row>
     <row r="31" ht="44.35" customHeight="1">
       <c r="B31" t="s" s="5">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C31" t="b" s="10">
         <v>1</v>
@@ -6886,7 +6955,7 @@
     </row>
     <row r="32" ht="56.35" customHeight="1">
       <c r="B32" t="s" s="5">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C32" t="b" s="6">
         <v>0</v>
@@ -6906,7 +6975,7 @@
     </row>
     <row r="33" ht="32.35" customHeight="1">
       <c r="B33" t="s" s="5">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C33" t="b" s="10">
         <v>0</v>
@@ -6918,7 +6987,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="b" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="b" s="10">
         <v>1</v>
@@ -6926,7 +6995,7 @@
     </row>
     <row r="34" ht="20.35" customHeight="1">
       <c r="B34" t="s" s="5">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C34" t="b" s="6">
         <v>1</v>
@@ -6946,7 +7015,7 @@
     </row>
     <row r="35" ht="32.35" customHeight="1">
       <c r="B35" t="s" s="5">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C35" t="b" s="10">
         <v>0</v>
@@ -6966,7 +7035,7 @@
     </row>
     <row r="36" ht="44.35" customHeight="1">
       <c r="B36" t="s" s="5">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C36" t="b" s="6">
         <v>0</v>
@@ -6986,7 +7055,7 @@
     </row>
     <row r="37" ht="32.35" customHeight="1">
       <c r="B37" t="s" s="5">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C37" t="b" s="10">
         <v>0</v>
@@ -6998,15 +7067,15 @@
         <v>0</v>
       </c>
       <c r="F37" t="b" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" t="b" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" ht="32.35" customHeight="1">
       <c r="B38" t="s" s="5">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C38" t="b" s="6">
         <v>0</v>
@@ -7026,7 +7095,7 @@
     </row>
     <row r="39" ht="32.35" customHeight="1">
       <c r="B39" t="s" s="5">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C39" t="b" s="10">
         <v>1</v>
@@ -7046,7 +7115,7 @@
     </row>
     <row r="40" ht="32.35" customHeight="1">
       <c r="B40" t="s" s="5">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C40" t="b" s="6">
         <v>0</v>
@@ -7066,7 +7135,7 @@
     </row>
     <row r="41" ht="32.35" customHeight="1">
       <c r="B41" t="s" s="5">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C41" t="b" s="10">
         <v>1</v>
@@ -7086,7 +7155,7 @@
     </row>
     <row r="42" ht="20.35" customHeight="1">
       <c r="B42" t="s" s="5">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C42" t="b" s="6">
         <v>0</v>
@@ -7106,7 +7175,7 @@
     </row>
     <row r="43" ht="32.35" customHeight="1">
       <c r="B43" t="s" s="5">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C43" t="b" s="10">
         <v>1</v>
@@ -7126,7 +7195,7 @@
     </row>
     <row r="44" ht="32.35" customHeight="1">
       <c r="B44" t="s" s="5">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C44" t="b" s="6">
         <v>0</v>
@@ -7146,7 +7215,7 @@
     </row>
     <row r="45" ht="32.35" customHeight="1">
       <c r="B45" t="s" s="5">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C45" t="b" s="10">
         <v>0</v>
@@ -7166,7 +7235,7 @@
     </row>
     <row r="46" ht="32.35" customHeight="1">
       <c r="B46" t="s" s="5">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C46" t="b" s="6">
         <v>0</v>
@@ -7186,7 +7255,7 @@
     </row>
     <row r="47" ht="20.35" customHeight="1">
       <c r="B47" t="s" s="5">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C47" t="b" s="10">
         <v>0</v>
@@ -7206,7 +7275,7 @@
     </row>
     <row r="48" ht="32.35" customHeight="1">
       <c r="B48" t="s" s="5">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C48" t="b" s="6">
         <v>0</v>
@@ -7226,7 +7295,7 @@
     </row>
     <row r="49" ht="32.35" customHeight="1">
       <c r="B49" t="s" s="5">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C49" t="b" s="10">
         <v>0</v>
@@ -7246,7 +7315,7 @@
     </row>
     <row r="50" ht="20.35" customHeight="1">
       <c r="B50" t="s" s="5">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C50" t="b" s="6">
         <v>0</v>
@@ -7266,7 +7335,7 @@
     </row>
     <row r="51" ht="20.35" customHeight="1">
       <c r="B51" t="s" s="5">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C51" t="b" s="10">
         <v>1</v>
@@ -7286,7 +7355,7 @@
     </row>
     <row r="52" ht="32.35" customHeight="1">
       <c r="B52" t="s" s="5">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C52" t="b" s="6">
         <v>0</v>
@@ -7306,7 +7375,7 @@
     </row>
     <row r="53" ht="20.35" customHeight="1">
       <c r="B53" t="s" s="5">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C53" t="b" s="10">
         <v>1</v>
@@ -7326,7 +7395,7 @@
     </row>
     <row r="54" ht="20.35" customHeight="1">
       <c r="B54" t="s" s="5">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C54" t="b" s="6">
         <v>1</v>
@@ -7346,7 +7415,7 @@
     </row>
     <row r="55" ht="32.35" customHeight="1">
       <c r="B55" t="s" s="5">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C55" t="b" s="10">
         <v>0</v>
@@ -7366,7 +7435,7 @@
     </row>
     <row r="56" ht="32.35" customHeight="1">
       <c r="B56" t="s" s="5">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C56" t="b" s="6">
         <v>0</v>
@@ -7386,7 +7455,7 @@
     </row>
     <row r="57" ht="32.35" customHeight="1">
       <c r="B57" t="s" s="5">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C57" t="b" s="10">
         <v>1</v>
@@ -7406,10 +7475,10 @@
     </row>
     <row r="58" ht="20.35" customHeight="1">
       <c r="B58" t="s" s="5">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C58" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="b" s="6">
         <v>0</v>
@@ -7426,7 +7495,7 @@
     </row>
     <row r="59" ht="32.35" customHeight="1">
       <c r="B59" t="s" s="5">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C59" t="b" s="10">
         <v>0</v>
@@ -7446,7 +7515,7 @@
     </row>
     <row r="60" ht="32.35" customHeight="1">
       <c r="B60" t="s" s="5">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C60" t="b" s="6">
         <v>0</v>
@@ -7466,7 +7535,7 @@
     </row>
     <row r="61" ht="32.35" customHeight="1">
       <c r="B61" t="s" s="5">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C61" t="b" s="10">
         <v>1</v>
@@ -7486,7 +7555,7 @@
     </row>
     <row r="62" ht="20.35" customHeight="1">
       <c r="B62" t="s" s="5">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C62" t="b" s="6">
         <v>0</v>
@@ -7506,7 +7575,7 @@
     </row>
     <row r="63" ht="32.55" customHeight="1">
       <c r="B63" t="s" s="5">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C63" t="b" s="10">
         <v>0</v>
@@ -7518,7 +7587,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="b" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" t="b" s="10">
         <v>0</v>
@@ -7526,11 +7595,11 @@
     </row>
     <row r="64" ht="20.55" customHeight="1">
       <c r="B64" t="s" s="7">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C64" s="8">
         <f>COUNTIF(C4:C63,TRUE)/COUNTA(C4:C63)</f>
-        <v>0.45</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="D64" s="8">
         <f>COUNTIF(D4:D63,TRUE)/COUNTA(D4:D63)</f>
@@ -7542,20 +7611,20 @@
       </c>
       <c r="F64" s="8">
         <f>COUNTIF(F4:F63,TRUE)/COUNTA(F4:F63)</f>
-        <v>0.35</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G64" s="8">
         <f>COUNTIF(G4:G63,TRUE)/COUNTA(G4:G63)</f>
-        <v>0.25</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="65" ht="20.35" customHeight="1">
       <c r="B65" t="s" s="7">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C65" s="7">
         <f>COUNTIF(C4:C63,TRUE)</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D65" s="7">
         <f>COUNTIF(D4:D63,TRUE)</f>
@@ -7567,11 +7636,11 @@
       </c>
       <c r="F65" s="7">
         <f>COUNTIF(F4:F63,TRUE)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G65" s="7">
         <f>COUNTIF(G4:G63,TRUE)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>